<commit_message>
added solder paste to ADC center pad
</commit_message>
<xml_diff>
--- a/hardware/Project Outputs for OK6010_DB/Bill of Materials-OK6010_DB.xlsx
+++ b/hardware/Project Outputs for OK6010_DB/Bill of Materials-OK6010_DB.xlsx
@@ -1,20 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Al\altium\DigitalServo\Version07jun12\Project Outputs for OK6010_DB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="13395" windowHeight="10290"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22545" windowHeight="13395"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-OK6010_DB" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="309">
   <si>
     <t>Designator</t>
   </si>
@@ -226,7 +236,7 @@
     <t>445-6008-1-ND</t>
   </si>
   <si>
-    <t>C3216X5R0J107M</t>
+    <t>C3216X5R0J107M160AB</t>
   </si>
   <si>
     <t>C107, C108, C109, C110</t>
@@ -238,7 +248,7 @@
     <t>712-1328-1-ND</t>
   </si>
   <si>
-    <t>Johanson Technology Inc</t>
+    <t>Johanson Technology Inc.</t>
   </si>
   <si>
     <t>251R14S1R8BV4T</t>
@@ -265,7 +275,7 @@
     <t>ACX1426-ND</t>
   </si>
   <si>
-    <t>Amphenol Connex</t>
+    <t>Amphenol-RF Division</t>
   </si>
   <si>
     <t>132289</t>
@@ -286,7 +296,7 @@
     <t>A97594-ND</t>
   </si>
   <si>
-    <t>TE Connectivity</t>
+    <t>TE Connectivity AMP Connectors</t>
   </si>
   <si>
     <t>5-1814832-1</t>
@@ -325,7 +335,7 @@
     <t>WM2746-ND</t>
   </si>
   <si>
-    <t>Molex Inc</t>
+    <t>Molex, LLC</t>
   </si>
   <si>
     <t>0022292041</t>
@@ -445,7 +455,7 @@
     <t>RNCS0603BKE249RCT-ND</t>
   </si>
   <si>
-    <t>Stackpole Electronics Inc</t>
+    <t>Stackpole Electronics Inc.</t>
   </si>
   <si>
     <t>RNCS0603BKE249R</t>
@@ -772,13 +782,13 @@
     <t>MSOP10sm</t>
   </si>
   <si>
-    <t>IC AMP INST ICMOS LDRIFT 10MSOP, Programmable Gain Instumentation Amp</t>
+    <t>Programmable Gain Instumentation Amp, IC AMP INST ICMOS LDRIFT 10MSOP, IC AMP INST ICMOS LDRIFT 10MSOP, IC AMP INST ICMOS LDRIFT 10MSOP</t>
   </si>
   <si>
     <t>AD8251ARMZ-ND</t>
   </si>
   <si>
-    <t>Analog Devices Inc</t>
+    <t>Analog Devices Inc.</t>
   </si>
   <si>
     <t>AD8251ARMZ</t>
@@ -904,10 +914,7 @@
     <t>595-OPA453FAKTWT</t>
   </si>
   <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
-    <t>OPA453FAKTWT</t>
+    <t>Loading...</t>
   </si>
   <si>
     <t>U12</t>
@@ -949,7 +956,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -961,7 +968,7 @@
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
-      <name val="MS Sans Serif"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1012,25 +1019,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1042,6 +1037,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1058,44 +1056,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1123,14 +1121,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1158,6 +1173,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1169,166 +1201,142 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -1337,24 +1345,24 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1383,7 +1391,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1411,8 +1419,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1441,7 +1449,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1470,7 +1478,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1499,7 +1507,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1527,8 +1535,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1557,7 +1565,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1586,7 +1594,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1615,7 +1623,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1644,7 +1652,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1673,7 +1681,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1702,7 +1710,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1731,7 +1739,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1760,7 +1768,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1788,37 +1796,37 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="5">
         <v>16</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1847,7 +1855,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1876,7 +1884,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1905,7 +1913,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1934,7 +1942,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1963,7 +1971,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1992,7 +2000,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -2021,7 +2029,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -2049,8 +2057,8 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2078,8 +2086,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -2108,7 +2116,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2137,7 +2145,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -2166,7 +2174,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="2" t="s">
         <v>149</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -2194,8 +2202,8 @@
         <v>153</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -2224,7 +2232,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -2253,7 +2261,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="2" t="s">
         <v>163</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -2282,7 +2290,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="2" t="s">
         <v>167</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -2311,7 +2319,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="2" t="s">
         <v>171</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -2340,7 +2348,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2369,7 +2377,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -2398,7 +2406,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -2427,7 +2435,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2456,7 +2464,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -2485,7 +2493,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="2" t="s">
         <v>194</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -2514,7 +2522,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="2" t="s">
         <v>198</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -2543,7 +2551,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="2" t="s">
         <v>202</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -2572,7 +2580,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="2" t="s">
         <v>206</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -2601,7 +2609,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="2" t="s">
         <v>210</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -2630,7 +2638,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="2" t="s">
         <v>214</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -2659,7 +2667,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="2" t="s">
         <v>221</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -2688,7 +2696,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="2" t="s">
         <v>225</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -2717,7 +2725,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="2" t="s">
         <v>229</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -2746,7 +2754,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="2" t="s">
         <v>233</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -2775,7 +2783,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="2" t="s">
         <v>237</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -2804,7 +2812,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="2" t="s">
         <v>242</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -2833,7 +2841,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="2" t="s">
         <v>249</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -2862,7 +2870,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="2" t="s">
         <v>256</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -2891,7 +2899,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="2" t="s">
         <v>262</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -2920,7 +2928,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="2" t="s">
         <v>268</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -2949,7 +2957,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="2" t="s">
         <v>274</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -2978,7 +2986,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="2" t="s">
         <v>279</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -3007,7 +3015,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="2" t="s">
         <v>284</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -3036,7 +3044,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="2" t="s">
         <v>290</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -3061,21 +3069,21 @@
         <v>296</v>
       </c>
       <c r="I59" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+      <c r="B60" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="E60" s="3">
         <v>1</v>
@@ -3084,27 +3092,27 @@
         <v>13</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>254</v>
       </c>
       <c r="I60" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="B61" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>258</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E61" s="3">
         <v>5</v>
@@ -3113,13 +3121,13 @@
         <v>13</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>254</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>